<commit_message>
[refactor] update with crudpp
</commit_message>
<xml_diff>
--- a/Compliance One Issues List 2024 03 04.xlsx
+++ b/Compliance One Issues List 2024 03 04.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="56">
   <si>
     <t xml:space="preserve">Number</t>
   </si>
@@ -258,6 +258,10 @@
     <t xml:space="preserve">Add a Sanctions section to the form include:
 A button for "Is a US Person"
 A button for "Subject to Sanctions?" - this is ticked, then open to fields. The first "Sanctions Regime" and second, a free field text to describe the applicable sanctions. We should allow the user to add more "Sanctions Regime" and associated free field texts.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TBD (US person in company and Individual)
+List of saction regime to be defined</t>
   </si>
 </sst>
 </file>
@@ -657,7 +661,7 @@
   </sheetPr>
   <dimension ref="B1:F19"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A17" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E16" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="F19" activeCellId="0" sqref="F19"/>
     </sheetView>
   </sheetViews>
@@ -961,7 +965,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="99.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="105.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B19" s="6" t="n">
         <v>17</v>
       </c>
@@ -974,8 +978,8 @@
       <c r="E19" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="F19" s="1" t="s">
-        <v>27</v>
+      <c r="F19" s="9" t="s">
+        <v>55</v>
       </c>
     </row>
   </sheetData>

</xml_diff>